<commit_message>
fills in trap,recapture metadata tables
</commit_message>
<xml_diff>
--- a/data-raw/metadata/battle-recapture-metadata.xlsx
+++ b/data-raw/metadata/battle-recapture-metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Downloads/metadata template/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/edi-battle-clear-rst/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D68CA221-3B16-704B-A5F0-DE6707F29C7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79905E67-DD73-9241-A85F-DACD45B4A976}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" tabRatio="834" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33140" yWindow="-19920" windowWidth="30240" windowHeight="17100" tabRatio="834" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="9" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -74,6 +74,72 @@
   </si>
   <si>
     <t>attribute_name</t>
+  </si>
+  <si>
+    <t>site</t>
+  </si>
+  <si>
+    <t>release_id</t>
+  </si>
+  <si>
+    <t>date_recaptured</t>
+  </si>
+  <si>
+    <t>number_recaptured</t>
+  </si>
+  <si>
+    <t>median_fork_length_recaptured</t>
+  </si>
+  <si>
+    <t>Site where recapture samples were taken</t>
+  </si>
+  <si>
+    <t>Identifier of the released fish</t>
+  </si>
+  <si>
+    <t>Date fish was recaptured</t>
+  </si>
+  <si>
+    <t>Median fork length of the recaptured fish</t>
+  </si>
+  <si>
+    <t>nominal</t>
+  </si>
+  <si>
+    <t>enumerated</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>dateTime</t>
+  </si>
+  <si>
+    <t>ratio</t>
+  </si>
+  <si>
+    <t>numeric</t>
+  </si>
+  <si>
+    <t>count of fish</t>
+  </si>
+  <si>
+    <t>whole</t>
+  </si>
+  <si>
+    <t>millimeter</t>
+  </si>
+  <si>
+    <t>real</t>
+  </si>
+  <si>
+    <t>2004-01-15</t>
+  </si>
+  <si>
+    <t>2021-03-13</t>
+  </si>
+  <si>
+    <t>Number of fish recaptured</t>
   </si>
 </sst>
 </file>
@@ -128,7 +194,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -143,6 +209,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -231,7 +306,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -519,7 +594,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -530,7 +605,7 @@
   <dimension ref="A1:AMG10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -591,10 +666,115 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="J2" s="4"/>
       <c r="K2" s="2"/>
       <c r="L2" s="7"/>
+    </row>
+    <row r="3" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L4" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="M4" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="K5" s="8"/>
+      <c r="L5" s="10">
+        <v>0</v>
+      </c>
+      <c r="M5" s="10">
+        <v>1180</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="L6" s="5">
+        <v>33</v>
+      </c>
+      <c r="M6" s="5">
+        <v>79</v>
+      </c>
     </row>
     <row r="9" spans="1:13" ht="35.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
edits metadata tables and fills out make_metadata_xml.R
</commit_message>
<xml_diff>
--- a/data-raw/metadata/battle-recapture-metadata.xlsx
+++ b/data-raw/metadata/battle-recapture-metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/edi-battle-clear-rst/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79905E67-DD73-9241-A85F-DACD45B4A976}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB7708BB-3904-3E43-9F17-DF0977CEBDC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33140" yWindow="-19920" windowWidth="30240" windowHeight="17100" tabRatio="834" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -103,9 +103,6 @@
     <t>Median fork length of the recaptured fish</t>
   </si>
   <si>
-    <t>nominal</t>
-  </si>
-  <si>
     <t>enumerated</t>
   </si>
   <si>
@@ -140,6 +137,9 @@
   </si>
   <si>
     <t>Number of fish recaptured</t>
+  </si>
+  <si>
+    <t>ordinal</t>
   </si>
 </sst>
 </file>
@@ -194,7 +194,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -215,9 +215,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -605,7 +602,7 @@
   <dimension ref="A1:AMG10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C2" sqref="C2:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -674,10 +671,10 @@
         <v>21</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J2" s="4"/>
       <c r="K2" s="2"/>
@@ -691,10 +688,10 @@
         <v>22</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="34" x14ac:dyDescent="0.2">
@@ -705,16 +702,16 @@
         <v>23</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L4" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="M4" s="9" t="s">
         <v>35</v>
-      </c>
-      <c r="M4" s="9" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="51" x14ac:dyDescent="0.2">
@@ -722,28 +719,28 @@
         <v>19</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="G5" s="5" t="s">
+      <c r="H5" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="H5" s="5" t="s">
-        <v>32</v>
-      </c>
       <c r="K5" s="8"/>
-      <c r="L5" s="10">
+      <c r="L5" s="5">
         <v>0</v>
       </c>
-      <c r="M5" s="10">
+      <c r="M5" s="5">
         <v>1180</v>
       </c>
     </row>
@@ -755,19 +752,19 @@
         <v>24</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="F6" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G6" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" s="5" t="s">
         <v>33</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>34</v>
       </c>
       <c r="L6" s="5">
         <v>33</v>

</xml_diff>